<commit_message>
Grace ran v7 0816
</commit_message>
<xml_diff>
--- a/SDG Financing Simplified model (Egypt)/v7/output/modeloutput_arg.xlsx
+++ b/SDG Financing Simplified model (Egypt)/v7/output/modeloutput_arg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView yWindow="2085" windowWidth="17250" windowHeight="9945"/>
+    <workbookView windowWidth="17030" windowHeight="10730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -809,6 +809,1072 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Output per Capita</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$AD$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>7.20982246431157</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.51165500305661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.80230525418306</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.08208221002443</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.35232505233587</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.54260110515253</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.71120893745051</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.86016336390328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9934459504287</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.12359353837921</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.24256681995524</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.34525444294598</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.43260292598602</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.50494469286603</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.56410355938303</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.60745929998407</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.63271269037288</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.63664699890861</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.61515609918516</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.56834703086827</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.52869796520963</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.49627871163798</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.46632189201621</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.43592218761492</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.41330820149639</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.40053487121888</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.39596042834273</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.39832571928849</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.40637273967798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Consumption per Capita</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$AD$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1.67255654364453</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.89608761612348</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.11589634559938</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.33096019026934</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.54090478672517</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.72336992876161</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.89766475524438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.06369008173814</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.21986100162234</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.38011958840573</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.54261730594596</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7070072757861</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8753584295884</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.04982241074079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.23361103974185</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.42854363439577</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.6367562156703</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.86023034410433</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.05124474161192</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.05164848402238</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.05536698895539</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.06260930841179</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.06915809159993</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0725007371106</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.08064695779685</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.09560347462593</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.11672597718371</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.14180541983025</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.16929417386063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="187240386"/>
+        <c:axId val="533133178"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="187240386"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="533133178"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="533133178"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="187240386"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:externalData r:id="rId1">
+    <c:autoUpdate val="0"/>
+  </c:externalData>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4904740" y="2419350"/>
+        <a:ext cx="4585335" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1071,8 +2137,8 @@
   <sheetPr/>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66363636363636" defaultRowHeight="14"/>
@@ -1997,5 +3063,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>